<commit_message>
added updated on 15-10-2025
</commit_message>
<xml_diff>
--- a/testData/executeTestCaseTabTestData/executeTestCaseTab_testData.xlsx
+++ b/testData/executeTestCaseTabTestData/executeTestCaseTab_testData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MohitAman\Desktop\UAT_NEXTNEXT_BLAZE_FRAMEWORK_AUTO\testData\executeTestCaseTabTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7AD6D37-6B87-4D8E-ABCC-AEAAF177FD3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65097903-4D8F-4A27-9C8E-810F9EBC8118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -568,7 +568,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:K1048576"/>
+      <selection sqref="A1:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>

</xml_diff>

<commit_message>
tc018 and tc042 added
</commit_message>
<xml_diff>
--- a/testData/executeTestCaseTabTestData/executeTestCaseTab_testData.xlsx
+++ b/testData/executeTestCaseTabTestData/executeTestCaseTab_testData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6800" activeTab="7"/>
+    <workbookView windowWidth="19200" windowHeight="6080" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="tc002" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,8 @@
     <sheet name="tc021" sheetId="7" r:id="rId6"/>
     <sheet name="tc036" sheetId="8" r:id="rId7"/>
     <sheet name="tc037" sheetId="9" r:id="rId8"/>
+    <sheet name="tc018" sheetId="10" r:id="rId9"/>
+    <sheet name="tc042" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="39">
   <si>
     <t>Project Name</t>
   </si>
@@ -124,6 +126,33 @@
   </si>
   <si>
     <t>TestSuite 10</t>
+  </si>
+  <si>
+    <t>test run</t>
+  </si>
+  <si>
+    <t>defect Id</t>
+  </si>
+  <si>
+    <t>Mayukh_Release</t>
+  </si>
+  <si>
+    <t>Mayukh_TestCycle_Execute</t>
+  </si>
+  <si>
+    <t>Mayukh_Cycle_Execute</t>
+  </si>
+  <si>
+    <t>TR-143</t>
+  </si>
+  <si>
+    <t>DF-315</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>videomorethan6MB.mp4</t>
   </si>
 </sst>
 </file>
@@ -136,7 +165,7 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -148,15 +177,27 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
+      <sz val="8.2"/>
+      <color rgb="FF667084"/>
+      <name val="Arial"/>
       <charset val="134"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF475467"/>
+      <name val="Arial"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="8.25"/>
@@ -309,12 +350,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -627,144 +674,151 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1121,12 +1175,72 @@
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="5"/>
+  <cols>
+    <col min="6" max="6" width="19.3333333333333" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" ht="20" spans="1:6">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
 </file>
@@ -1206,36 +1320,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="7" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1260,54 +1374,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="8">
         <v>1</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="7" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1344,10 +1458,10 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C2" t="s">
@@ -1391,10 +1505,10 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C2" t="s">
@@ -1428,30 +1542,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="6" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1466,7 +1580,7 @@
   <sheetPr/>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -1479,31 +1593,88 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
+      <c r="A1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="5"/>
+  <sheetData>
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tc042 and tc051 added
</commit_message>
<xml_diff>
--- a/testData/executeTestCaseTabTestData/executeTestCaseTab_testData.xlsx
+++ b/testData/executeTestCaseTabTestData/executeTestCaseTab_testData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6080" activeTab="9"/>
+    <workbookView windowWidth="19200" windowHeight="6080" firstSheet="1" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="tc002" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="tc037" sheetId="9" r:id="rId8"/>
     <sheet name="tc018" sheetId="10" r:id="rId9"/>
     <sheet name="tc042" sheetId="11" r:id="rId10"/>
+    <sheet name="tc043" sheetId="12" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="40">
   <si>
     <t>Project Name</t>
   </si>
@@ -153,6 +154,9 @@
   </si>
   <si>
     <t>videomorethan6MB.mp4</t>
+  </si>
+  <si>
+    <t>TR-10000</t>
   </si>
 </sst>
 </file>
@@ -181,17 +185,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="8.2"/>
       <color rgb="FF667084"/>
       <name val="Arial"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
@@ -808,13 +812,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1190,7 +1194,7 @@
   <sheetPr/>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -1200,43 +1204,88 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
+      <c r="A1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="3"/>
+  <sheetData>
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" ht="20" spans="1:6">
-      <c r="A2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>38</v>
+      <c r="D2" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1320,36 +1369,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="3" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1374,54 +1423,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G2" s="8">
         <v>1</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="3" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1458,10 +1507,10 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C2" t="s">
@@ -1505,10 +1554,10 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C2" t="s">
@@ -1542,30 +1591,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1593,30 +1642,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1638,19 +1687,19 @@
   <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="5"/>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>30</v>
       </c>
       <c r="F1" t="s">
@@ -1658,22 +1707,22 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="7" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added TC050 added data
</commit_message>
<xml_diff>
--- a/testData/executeTestCaseTabTestData/executeTestCaseTab_testData.xlsx
+++ b/testData/executeTestCaseTabTestData/executeTestCaseTab_testData.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MohitAman\Desktop\UAT_NEXTNEXT_BLAZE_FRAMEWORK_AUTO\testData\executeTestCaseTabTestData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9F4A2E6-F5F4-4012-A223-800DA5A271A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="18600" windowHeight="6080" firstSheet="1" activeTab="10"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tc002" sheetId="1" r:id="rId1"/>
@@ -18,26 +24,14 @@
     <sheet name="tc018" sheetId="10" r:id="rId9"/>
     <sheet name="tc042" sheetId="11" r:id="rId10"/>
     <sheet name="tc029" sheetId="12" r:id="rId11"/>
+    <sheet name="tc050" sheetId="13" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="63">
   <si>
     <t>Project Name</t>
   </si>
@@ -231,14 +225,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="25">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -257,11 +245,10 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8.2"/>
+      <sz val="8.1999999999999993"/>
       <color rgb="FF667084"/>
       <name val="Arial"/>
       <charset val="134"/>
@@ -279,151 +266,13 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Aptos Narrow"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Aptos Narrow"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Aptos Narrow"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Aptos Narrow"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Aptos Narrow"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Aptos Narrow"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Aptos Narrow"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Aptos Narrow"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Aptos Narrow"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Aptos Narrow"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Aptos Narrow"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Aptos Narrow"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Aptos Narrow"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Aptos Narrow"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Aptos Narrow"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Aptos Narrow"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Aptos Narrow"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -436,194 +285,8 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -631,253 +294,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -890,62 +311,22 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Currency" xfId="2" builtinId="4"/>
-    <cellStyle name="Percent" xfId="3" builtinId="5"/>
-    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Link" xfId="6" builtinId="8"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
-    <cellStyle name="Note" xfId="8" builtinId="10"/>
-    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
-    <cellStyle name="Title" xfId="10" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
-    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
-    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
-    <cellStyle name="Input" xfId="16" builtinId="20"/>
-    <cellStyle name="Output" xfId="17" builtinId="21"/>
-    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
-    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
-    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
-    <cellStyle name="Total" xfId="21" builtinId="25"/>
-    <cellStyle name="Good" xfId="22" builtinId="26"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
-    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1223,21 +604,21 @@
       </a:style>
     </a:lnDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="22.9083333333333" customWidth="1"/>
+    <col min="1" max="1" width="22.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -1252,25 +633,23 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14"/>
   <cols>
-    <col min="6" max="6" width="19.3333333333333" customWidth="1"/>
+    <col min="6" max="6" width="19.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" ht="15">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1312,20 +691,18 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="2" width="21" customWidth="1"/>
   </cols>
@@ -1414,25 +791,90 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{552C4795-9F9A-412F-827B-3989E17F0C7B}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15">
+      <c r="A1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15">
+      <c r="A2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="9">
+        <v>1</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:B2"/>
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.725" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="27.1833333333333" customWidth="1"/>
-    <col min="2" max="2" width="25.0916666666667" customWidth="1"/>
-    <col min="3" max="3" width="24.5416666666667" customWidth="1"/>
-    <col min="4" max="4" width="24.8166666666667" customWidth="1"/>
+    <col min="1" max="1" width="27.1796875" customWidth="1"/>
+    <col min="2" max="2" width="25.08984375" customWidth="1"/>
+    <col min="3" max="3" width="24.54296875" customWidth="1"/>
+    <col min="4" max="4" width="24.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1471,25 +913,23 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:E2"/>
+      <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="48.6333333333333" customWidth="1"/>
-    <col min="2" max="2" width="33.6333333333333" customWidth="1"/>
-    <col min="3" max="3" width="27.0916666666667" customWidth="1"/>
-    <col min="4" max="4" width="22.6333333333333" customWidth="1"/>
+    <col min="1" max="1" width="48.6328125" customWidth="1"/>
+    <col min="2" max="2" width="33.6328125" customWidth="1"/>
+    <col min="3" max="3" width="27.08984375" customWidth="1"/>
+    <col min="4" max="4" width="22.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1528,22 +968,20 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I$1:K$1048576"/>
+      <selection activeCell="I1" sqref="I1:K1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="8" max="8" width="28.8166666666667" customWidth="1"/>
+    <col min="8" max="8" width="28.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1600,23 +1038,21 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:C2"/>
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="28.75" customWidth="1"/>
-    <col min="2" max="2" width="19.75" customWidth="1"/>
+    <col min="1" max="1" width="28.7265625" customWidth="1"/>
+    <col min="2" max="2" width="19.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1630,7 +1066,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" ht="15">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1643,24 +1079,22 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:D2"/>
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="29.4166666666667" customWidth="1"/>
-    <col min="2" max="2" width="16.5833333333333" customWidth="1"/>
-    <col min="3" max="3" width="11.5" customWidth="1"/>
+    <col min="1" max="1" width="29.453125" customWidth="1"/>
+    <col min="2" max="2" width="16.54296875" customWidth="1"/>
+    <col min="3" max="3" width="11.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1677,7 +1111,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" ht="15">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1693,28 +1127,26 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:D2"/>
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="37.3333333333333" customWidth="1"/>
-    <col min="2" max="2" width="21.5833333333333" customWidth="1"/>
-    <col min="3" max="3" width="17.9166666666667" customWidth="1"/>
-    <col min="4" max="4" width="22.1666666666667" customWidth="1"/>
+    <col min="1" max="1" width="37.36328125" customWidth="1"/>
+    <col min="2" max="2" width="21.54296875" customWidth="1"/>
+    <col min="3" max="3" width="17.90625" customWidth="1"/>
+    <col min="4" max="4" width="22.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" ht="15">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -1728,7 +1160,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" ht="15">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1744,28 +1176,26 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="34.9166666666667" customWidth="1"/>
-    <col min="2" max="2" width="26.25" customWidth="1"/>
-    <col min="3" max="3" width="23.0833333333333" customWidth="1"/>
-    <col min="4" max="4" width="28.9166666666667" customWidth="1"/>
+    <col min="1" max="1" width="34.90625" customWidth="1"/>
+    <col min="2" max="2" width="26.26953125" customWidth="1"/>
+    <col min="3" max="3" width="23.08984375" customWidth="1"/>
+    <col min="4" max="4" width="28.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" ht="15">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -1779,7 +1209,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" ht="15">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1795,20 +1225,18 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
@@ -1852,6 +1280,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added tc20 for execute tab
</commit_message>
<xml_diff>
--- a/testData/executeTestCaseTabTestData/executeTestCaseTab_testData.xlsx
+++ b/testData/executeTestCaseTabTestData/executeTestCaseTab_testData.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MohitAman\Desktop\UAT_NEXTNEXT_BLAZE_FRAMEWORK_AUTO\testData\executeTestCaseTabTestData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9083473-902F-4DA9-86BC-3036F75F53BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6800" firstSheet="26" activeTab="35"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="27" activeTab="36" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tc001" sheetId="1" r:id="rId1"/>
@@ -43,26 +49,14 @@
     <sheet name="tc050" sheetId="36" r:id="rId34"/>
     <sheet name="tc044" sheetId="37" r:id="rId35"/>
     <sheet name="tc029" sheetId="38" r:id="rId36"/>
+    <sheet name="tc020" sheetId="40" r:id="rId37"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="89">
   <si>
     <t>projectName</t>
   </si>
@@ -334,14 +328,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="25">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -369,7 +357,7 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="8.2"/>
+      <sz val="8.1999999999999993"/>
       <color rgb="FF667084"/>
       <name val="Arial"/>
       <charset val="134"/>
@@ -380,152 +368,8 @@
       <name val="Arial"/>
       <charset val="1"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Aptos Narrow"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Aptos Narrow"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Aptos Narrow"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Aptos Narrow"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Aptos Narrow"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Aptos Narrow"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Aptos Narrow"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Aptos Narrow"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Aptos Narrow"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Aptos Narrow"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Aptos Narrow"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Aptos Narrow"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Aptos Narrow"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Aptos Narrow"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Aptos Narrow"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Aptos Narrow"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Aptos Narrow"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="34">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -538,194 +382,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -733,253 +391,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -989,7 +405,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -999,61 +414,17 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Currency" xfId="2" builtinId="4"/>
-    <cellStyle name="Percent" xfId="3" builtinId="5"/>
-    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Link" xfId="6" builtinId="8"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
-    <cellStyle name="Note" xfId="8" builtinId="10"/>
-    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
-    <cellStyle name="Title" xfId="10" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
-    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
-    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
-    <cellStyle name="Input" xfId="16" builtinId="20"/>
-    <cellStyle name="Output" xfId="17" builtinId="21"/>
-    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
-    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
-    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
-    <cellStyle name="Total" xfId="21" builtinId="25"/>
-    <cellStyle name="Good" xfId="22" builtinId="26"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
-    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1331,21 +702,19 @@
       </a:style>
     </a:lnDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="1"/>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="22.575" customWidth="1"/>
+    <col min="1" max="1" width="22.54296875" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1367,69 +736,65 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="38.7083333333333" customWidth="1"/>
-    <col min="2" max="2" width="17.8583333333333" customWidth="1"/>
+    <col min="1" max="1" width="38.7265625" customWidth="1"/>
+    <col min="2" max="2" width="17.81640625" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="7" t="s">
+      <c r="A2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>42</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="28.425" customWidth="1"/>
-    <col min="2" max="2" width="31.2833333333333" customWidth="1"/>
+    <col min="1" max="1" width="28.453125" customWidth="1"/>
+    <col min="2" max="2" width="31.26953125" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
-    <col min="4" max="4" width="28.575" customWidth="1"/>
+    <col min="4" max="4" width="28.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1468,96 +833,92 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:H2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="7"/>
+      <selection sqref="A1:H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="26.575" customWidth="1"/>
-    <col min="7" max="7" width="32.575" customWidth="1"/>
-    <col min="8" max="8" width="29.7083333333333" customWidth="1"/>
+    <col min="1" max="1" width="26.54296875" customWidth="1"/>
+    <col min="7" max="7" width="32.54296875" customWidth="1"/>
+    <col min="8" max="8" width="29.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="5">
         <v>1</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="1" t="s">
         <v>48</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="7"/>
-  <sheetData>
-    <row r="1" ht="14.5" spans="1:8">
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -1583,7 +944,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" ht="14.5" spans="1:8">
+    <row r="2" spans="1:8" ht="15">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1611,103 +972,99 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="1" t="s">
         <v>50</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="3" max="3" width="20.425" customWidth="1"/>
-    <col min="4" max="4" width="18.425" customWidth="1"/>
+    <col min="3" max="3" width="20.453125" customWidth="1"/>
+    <col min="4" max="4" width="18.453125" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>37</v>
       </c>
       <c r="F1" t="s">
@@ -1715,59 +1072,57 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="7" t="s">
+      <c r="A2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="8" t="s">
         <v>52</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="B1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col min="6" max="6" width="28" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>37</v>
       </c>
       <c r="F1" t="s">
@@ -1775,199 +1130,189 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="8" t="s">
-        <v>2</v>
+      <c r="A2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <cols>
+    <col min="1" max="1" width="19.26953125" customWidth="1"/>
+    <col min="2" max="2" width="25.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+      <c r="D2" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="3"/>
+      <selection sqref="A1:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="19.2833333333333" customWidth="1"/>
-    <col min="2" max="2" width="25.1333333333333" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="3"/>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="$A1:$XFD2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="3"/>
-  <cols>
-    <col min="1" max="1" width="36.575" customWidth="1"/>
+    <col min="1" max="1" width="36.54296875" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="14.575" customWidth="1"/>
+    <col min="3" max="3" width="14.54296875" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="7" t="s">
+      <c r="A2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>57</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="3"/>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="18.8583333333333" customWidth="1"/>
-    <col min="2" max="2" width="19.8583333333333" customWidth="1"/>
+    <col min="1" max="1" width="18.81640625" customWidth="1"/>
+    <col min="2" max="2" width="19.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D1" t="s">
@@ -1975,13 +1320,13 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="7" t="s">
+      <c r="A2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D2" t="s">
@@ -1990,32 +1335,30 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="$A1:$XFD2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="14" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="5"/>
+      <selection sqref="A1:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14" defaultRowHeight="14"/>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>58</v>
       </c>
       <c r="E1" t="s">
@@ -2026,16 +1369,16 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="7" t="s">
+      <c r="A2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>61</v>
       </c>
       <c r="E2" t="s">
@@ -2047,32 +1390,30 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.1333333333333" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="17.08984375" defaultRowHeight="14"/>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>58</v>
       </c>
       <c r="E1" t="s">
@@ -2083,16 +1424,16 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="7" t="s">
+      <c r="A2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>61</v>
       </c>
       <c r="E2" t="s">
@@ -2104,32 +1445,30 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="23.575" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="23.54296875" defaultRowHeight="14"/>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>58</v>
       </c>
       <c r="E1" t="s">
@@ -2140,16 +1479,16 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="7" t="s">
+      <c r="A2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>61</v>
       </c>
       <c r="E2" t="s">
@@ -2161,31 +1500,29 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="28.425" customWidth="1"/>
-    <col min="2" max="2" width="18.1333333333333" customWidth="1"/>
-    <col min="3" max="3" width="18.425" customWidth="1"/>
+    <col min="1" max="1" width="28.453125" customWidth="1"/>
+    <col min="2" max="2" width="18.08984375" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -2193,10 +1530,10 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>65</v>
       </c>
       <c r="C2" t="s">
@@ -2205,47 +1542,45 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1"/>
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="8" max="8" width="31.425" customWidth="1"/>
+    <col min="8" max="8" width="31.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="1" t="s">
         <v>46</v>
       </c>
       <c r="I1" t="s">
@@ -2253,28 +1588,28 @@
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="5">
         <v>1</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="1" t="s">
         <v>48</v>
       </c>
       <c r="I2">
@@ -2283,178 +1618,170 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="3"/>
+      <selection sqref="A1:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="27.7083333333333" customWidth="1"/>
-    <col min="2" max="2" width="19.425" customWidth="1"/>
-    <col min="3" max="3" width="21.1333333333333" customWidth="1"/>
-    <col min="4" max="4" width="17.425" customWidth="1"/>
+    <col min="1" max="1" width="27.7265625" customWidth="1"/>
+    <col min="2" max="2" width="19.453125" customWidth="1"/>
+    <col min="3" max="3" width="21.08984375" customWidth="1"/>
+    <col min="4" max="4" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="7" t="s">
+      <c r="A2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="1" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="1" t="s">
         <v>47</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="28.575" customWidth="1"/>
-    <col min="2" max="2" width="16.7083333333333" customWidth="1"/>
+    <col min="1" max="1" width="28.54296875" customWidth="1"/>
+    <col min="2" max="2" width="16.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>38</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="2" max="2" width="15.8583333333333" customWidth="1"/>
-    <col min="3" max="3" width="15.2833333333333" customWidth="1"/>
-    <col min="4" max="4" width="11.425" customWidth="1"/>
-    <col min="5" max="5" width="27.1333333333333" customWidth="1"/>
+    <col min="2" max="2" width="15.81640625" customWidth="1"/>
+    <col min="3" max="3" width="15.26953125" customWidth="1"/>
+    <col min="4" max="4" width="11.453125" customWidth="1"/>
+    <col min="5" max="5" width="27.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -2468,10 +1795,10 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C2" t="s">
@@ -2486,25 +1813,23 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="$A1:$XFD2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="5"/>
+      <selection sqref="A1:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="12.425" customWidth="1"/>
-    <col min="3" max="3" width="12.2833333333333" customWidth="1"/>
-    <col min="4" max="4" width="12.575" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" customWidth="1"/>
+    <col min="3" max="3" width="12.26953125" customWidth="1"/>
+    <col min="4" max="4" width="12.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2527,7 +1852,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" ht="28">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -2549,37 +1874,35 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="2" width="18.575" customWidth="1"/>
-    <col min="3" max="3" width="15.1333333333333" customWidth="1"/>
-    <col min="4" max="4" width="13.1333333333333" customWidth="1"/>
+    <col min="1" max="2" width="18.54296875" customWidth="1"/>
+    <col min="3" max="3" width="15.08984375" customWidth="1"/>
+    <col min="4" max="4" width="13.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E1" t="s">
@@ -2587,38 +1910,36 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="7" t="s">
+      <c r="A2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="1" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="$A1:$XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="24.1333333333333" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="5"/>
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="24.08984375" defaultRowHeight="14"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
@@ -2640,7 +1961,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" ht="28" spans="1:6">
+    <row r="2" spans="1:6" ht="28">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -2662,219 +1983,209 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="1" t="s">
         <v>82</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="4"/>
+      <selection sqref="A1:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="1" t="s">
         <v>44</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:H2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="7"/>
+      <selection sqref="A1:H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="5">
         <v>1</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="1" t="s">
         <v>48</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="7"/>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="29.8583333333333" customWidth="1"/>
+    <col min="1" max="1" width="29.81640625" customWidth="1"/>
     <col min="2" max="2" width="28" customWidth="1"/>
-    <col min="3" max="3" width="26.8583333333333" customWidth="1"/>
-    <col min="4" max="5" width="22.7083333333333" customWidth="1"/>
-    <col min="6" max="6" width="18.7083333333333" customWidth="1"/>
-    <col min="8" max="8" width="42.8583333333333" customWidth="1"/>
+    <col min="3" max="3" width="26.81640625" customWidth="1"/>
+    <col min="4" max="5" width="22.7265625" customWidth="1"/>
+    <col min="6" max="6" width="18.7265625" customWidth="1"/>
+    <col min="8" max="8" width="42.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.5" spans="1:8">
+    <row r="1" spans="1:8" ht="15">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -2900,7 +2211,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" ht="14.5" spans="1:8">
+    <row r="2" spans="1:8" ht="15">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -2928,22 +2239,20 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="3"/>
-  <sheetData>
-    <row r="1" ht="28" spans="1:4">
+  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14"/>
+  <sheetData>
+    <row r="1" spans="1:4" ht="28">
       <c r="A1" s="2" t="s">
         <v>23</v>
       </c>
@@ -2957,7 +2266,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" ht="56" spans="1:4">
+    <row r="2" spans="1:4" ht="56">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -2973,20 +2282,18 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
@@ -3012,108 +2319,147 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F866ADB7-3A51-4F67-9A5C-24EF6D7D95EB}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="4"/>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="19.8583333333333" customWidth="1"/>
-    <col min="2" max="2" width="15.7083333333333" customWidth="1"/>
-    <col min="3" max="3" width="18.7083333333333" customWidth="1"/>
-    <col min="4" max="4" width="17.575" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+    <col min="2" max="2" width="15.7265625" customWidth="1"/>
+    <col min="3" max="3" width="18.7265625" customWidth="1"/>
+    <col min="4" max="4" width="17.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5">
+      <c r="A2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
       <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="2"/>
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="28.7083333333333" customWidth="1"/>
-    <col min="2" max="2" width="23.575" customWidth="1"/>
-    <col min="3" max="3" width="20.7083333333333" customWidth="1"/>
+    <col min="1" max="1" width="28.7265625" customWidth="1"/>
+    <col min="2" max="2" width="23.54296875" customWidth="1"/>
+    <col min="3" max="3" width="20.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -3140,25 +2486,23 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="3"/>
+      <selection sqref="A1:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="32.1333333333333" customWidth="1"/>
-    <col min="2" max="2" width="19.2833333333333" customWidth="1"/>
-    <col min="3" max="3" width="16.425" customWidth="1"/>
-    <col min="4" max="4" width="14.2833333333333" customWidth="1"/>
+    <col min="1" max="1" width="32.08984375" customWidth="1"/>
+    <col min="2" max="2" width="19.26953125" customWidth="1"/>
+    <col min="3" max="3" width="16.453125" customWidth="1"/>
+    <col min="4" max="4" width="14.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3191,26 +2535,24 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="38.8583333333333" customWidth="1"/>
-    <col min="2" max="2" width="36.8583333333333" customWidth="1"/>
+    <col min="1" max="1" width="38.81640625" customWidth="1"/>
+    <col min="2" max="2" width="36.81640625" customWidth="1"/>
     <col min="3" max="3" width="31" customWidth="1"/>
-    <col min="4" max="4" width="28.575" customWidth="1"/>
-    <col min="5" max="5" width="19.1333333333333" customWidth="1"/>
+    <col min="4" max="4" width="28.54296875" customWidth="1"/>
+    <col min="5" max="5" width="19.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -3249,57 +2591,54 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="7" t="s">
+      <c r="A2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>41</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added tc10 for execute tab
</commit_message>
<xml_diff>
--- a/testData/executeTestCaseTabTestData/executeTestCaseTab_testData.xlsx
+++ b/testData/executeTestCaseTabTestData/executeTestCaseTab_testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MohitAman\Desktop\UAT_NEXTNEXT_BLAZE_FRAMEWORK_AUTO\testData\executeTestCaseTabTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4416B94-9BC3-4994-A768-9393C8CB298C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96BCBB96-8DD0-4091-B959-437132E68C42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="27" activeTab="36" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="28" activeTab="37" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tc001" sheetId="1" r:id="rId1"/>
@@ -50,13 +50,14 @@
     <sheet name="tc044" sheetId="37" r:id="rId35"/>
     <sheet name="tc029" sheetId="38" r:id="rId36"/>
     <sheet name="tc020" sheetId="40" r:id="rId37"/>
+    <sheet name="tc010" sheetId="42" r:id="rId38"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="91">
   <si>
     <t>projectName</t>
   </si>
@@ -325,10 +326,10 @@
     <t>New Release 123</t>
   </si>
   <si>
-    <t>defif</t>
-  </si>
-  <si>
     <t>DF-317</t>
+  </si>
+  <si>
+    <t>defid</t>
   </si>
 </sst>
 </file>
@@ -2332,8 +2333,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F866ADB7-3A51-4F67-9A5C-24EF6D7D95EB}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -2355,7 +2356,7 @@
         <v>43</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -2375,7 +2376,56 @@
         <v>44</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0169DB9D-2F56-481E-A164-61CBB8B25DFD}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added tc41 for execute tab
</commit_message>
<xml_diff>
--- a/testData/executeTestCaseTabTestData/executeTestCaseTab_testData.xlsx
+++ b/testData/executeTestCaseTabTestData/executeTestCaseTab_testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MohitAman\Desktop\UAT_NEXTNEXT_BLAZE_FRAMEWORK_AUTO\testData\executeTestCaseTabTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96BCBB96-8DD0-4091-B959-437132E68C42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{920EF647-20C6-4694-A7BE-08D47EF50AD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="28" activeTab="37" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="28" activeTab="38" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tc001" sheetId="1" r:id="rId1"/>
@@ -51,13 +51,14 @@
     <sheet name="tc029" sheetId="38" r:id="rId36"/>
     <sheet name="tc020" sheetId="40" r:id="rId37"/>
     <sheet name="tc010" sheetId="42" r:id="rId38"/>
+    <sheet name="tc041" sheetId="43" r:id="rId39"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="95">
   <si>
     <t>projectName</t>
   </si>
@@ -330,6 +331,18 @@
   </si>
   <si>
     <t>defid</t>
+  </si>
+  <si>
+    <t>fileaddress</t>
+  </si>
+  <si>
+    <t>summary</t>
+  </si>
+  <si>
+    <t>testing</t>
+  </si>
+  <si>
+    <t>C:\Users\MohitAman\Documents\sheet 1.xlsx</t>
   </si>
 </sst>
 </file>
@@ -2388,7 +2401,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0169DB9D-2F56-481E-A164-61CBB8B25DFD}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -2426,6 +2439,73 @@
       </c>
       <c r="E2" s="1" t="s">
         <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14DB17CC-6B2B-4335-9FAC-602C559A2334}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>